<commit_message>
Calculator with upating result value to excel sheet
</commit_message>
<xml_diff>
--- a/Sudha/CalculatorRE_Queues/Data/Input/input.xlsx
+++ b/Sudha/CalculatorRE_Queues/Data/Input/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\UiPath\RPA-Developer-in-30-Days\RPA-Developer-in-30-Days\Sudha\CalculatorRE_Queues\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F627B2C1-37C3-4B8C-9256-18DB50140898}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C64FF0A-37C9-48D4-B83C-C8A015E97854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -366,7 +366,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D2" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>